<commit_message>
add compare func to HTMLtestRunner && test result
</commit_message>
<xml_diff>
--- a/smoothmodel_output/picker_compare/picker_compare.xlsx
+++ b/smoothmodel_output/picker_compare/picker_compare.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="619">
   <si>
     <t>掉帧率得分</t>
   </si>
@@ -1864,6 +1864,128 @@
   </si>
   <si>
     <t>平均分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.75% (112 /953)</t>
+  </si>
+  <si>
+    <t>10.07% (96/953)</t>
+  </si>
+  <si>
+    <t>0.00%
+ (0 /953)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.78%
+ (36 /953)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.59% (34/946)</t>
+  </si>
+  <si>
+    <t>11.84% (112 /946)</t>
+  </si>
+  <si>
+    <t>9.51% (90/946)</t>
+  </si>
+  <si>
+    <t>0.21%
+ (2 /946)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2.96%
+ (28 /946)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.97% (38/957)</t>
+  </si>
+  <si>
+    <t>11.49% (110 /957)</t>
+  </si>
+  <si>
+    <t>9.40% (90/957)</t>
+  </si>
+  <si>
+    <t>0.00% 
+(0 /957)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.45% 
+(33 /957)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.29% (107 /948)</t>
+  </si>
+  <si>
+    <t>0.00% (0/948)</t>
+  </si>
+  <si>
+    <t>9.92% (94/948)</t>
+  </si>
+  <si>
+    <t>0.00% 
+(0 /948)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.59%
+ (34 /948)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.90% (37/948)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3.78% (36/953)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11.83% (112 /947)</t>
+  </si>
+  <si>
+    <t>0.00% (0/947)</t>
+  </si>
+  <si>
+    <t>9.19% (87/947)</t>
+  </si>
+  <si>
+    <t>0.00% (0 /947)</t>
+  </si>
+  <si>
+    <t>3.80% (36 /947)</t>
+  </si>
+  <si>
+    <t>3.91% (37/947)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>With Picker</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>With Picker
+systemui 修改版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉通知栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下拉通知栏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No Picker
+systemui 修改版本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1982,7 +2104,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2066,13 +2188,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2154,7 +2296,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2172,6 +2314,9 @@
     <xf numFmtId="2" fontId="9" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="9" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2181,13 +2326,13 @@
     <xf numFmtId="2" fontId="9" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2199,16 +2344,22 @@
     <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2491,10 +2642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:L135"/>
+  <dimension ref="A3:L146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2546,13 +2697,13 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="43" t="s">
         <v>265</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="43">
         <f>AVERAGE(D4+D5)</f>
         <v>47.457999999999998</v>
       </c>
@@ -2585,9 +2736,9 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
+      <c r="A5" s="27"/>
+      <c r="B5" s="43"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="8"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
@@ -2599,11 +2750,11 @@
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="36"/>
-      <c r="B6" s="38" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="43">
         <f>AVERAGE(D6,D7)</f>
         <v>49.590249999999997</v>
       </c>
@@ -2636,9 +2787,9 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="36"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="37"/>
+      <c r="A7" s="27"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="18">
         <v>48.584499999999998</v>
       </c>
@@ -2668,7 +2819,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="27" t="s">
         <v>93</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2704,7 +2855,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="36"/>
+      <c r="A9" s="27"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
       <c r="D9" s="8"/>
@@ -2718,7 +2869,7 @@
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="36"/>
+      <c r="A10" s="27"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
       <c r="D10" s="2">
@@ -2750,7 +2901,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="36"/>
+      <c r="A11" s="27"/>
       <c r="B11" s="12" t="s">
         <v>102</v>
       </c>
@@ -2787,7 +2938,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="36" t="s">
+      <c r="A12" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2823,7 +2974,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="36"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
       <c r="D13" s="8"/>
@@ -2837,7 +2988,7 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="36"/>
+      <c r="A14" s="27"/>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="2">
@@ -2869,7 +3020,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="36"/>
+      <c r="A15" s="27"/>
       <c r="B15" s="12" t="s">
         <v>102</v>
       </c>
@@ -2903,7 +3054,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="27" t="s">
         <v>95</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2939,7 +3090,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="36"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="8"/>
@@ -2953,7 +3104,7 @@
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="36"/>
+      <c r="A18" s="27"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
       <c r="D18" s="13">
@@ -2985,7 +3136,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="36"/>
+      <c r="A19" s="27"/>
       <c r="B19" s="12" t="s">
         <v>102</v>
       </c>
@@ -3019,7 +3170,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="27" t="s">
         <v>108</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -3055,7 +3206,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="36"/>
+      <c r="A21" s="27"/>
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="8"/>
@@ -3069,7 +3220,7 @@
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="36"/>
+      <c r="A22" s="27"/>
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="2">
@@ -3101,7 +3252,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="36"/>
+      <c r="A23" s="27"/>
       <c r="B23" s="12" t="s">
         <v>102</v>
       </c>
@@ -3135,7 +3286,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="27" t="s">
         <v>110</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -3171,7 +3322,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="36"/>
+      <c r="A25" s="27"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
       <c r="D25" s="8"/>
@@ -3185,7 +3336,7 @@
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="36"/>
+      <c r="A26" s="27"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="2">
@@ -3217,7 +3368,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="36"/>
+      <c r="A27" s="27"/>
       <c r="B27" s="10" t="s">
         <v>102</v>
       </c>
@@ -3251,7 +3402,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="27" t="s">
         <v>141</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -3287,7 +3438,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="36"/>
+      <c r="A29" s="27"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
       <c r="D29" s="8"/>
@@ -3301,7 +3452,7 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="36"/>
+      <c r="A30" s="27"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
       <c r="D30" s="2">
@@ -3333,7 +3484,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="36"/>
+      <c r="A31" s="27"/>
       <c r="B31" s="10" t="s">
         <v>102</v>
       </c>
@@ -3367,7 +3518,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="27" t="s">
         <v>142</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -3403,7 +3554,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="36"/>
+      <c r="A33" s="27"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
       <c r="D33" s="8"/>
@@ -3417,7 +3568,7 @@
       <c r="L33" s="9"/>
     </row>
     <row r="34" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="36"/>
+      <c r="A34" s="27"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
       <c r="D34" s="2">
@@ -3449,7 +3600,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="36"/>
+      <c r="A35" s="27"/>
       <c r="B35" s="12" t="s">
         <v>102</v>
       </c>
@@ -3483,7 +3634,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="36" t="s">
+      <c r="A36" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B36" s="12" t="s">
@@ -3519,7 +3670,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="36"/>
+      <c r="A37" s="27"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="8"/>
@@ -3533,7 +3684,7 @@
       <c r="L37" s="9"/>
     </row>
     <row r="38" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="36"/>
+      <c r="A38" s="27"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
       <c r="D38" s="2">
@@ -3565,7 +3716,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="36"/>
+      <c r="A39" s="27"/>
       <c r="B39" s="12" t="s">
         <v>102</v>
       </c>
@@ -3599,7 +3750,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="27" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -3635,7 +3786,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="36"/>
+      <c r="A41" s="27"/>
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="8"/>
@@ -3649,11 +3800,11 @@
       <c r="L41" s="9"/>
     </row>
     <row r="42" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="36"/>
-      <c r="B42" s="34" t="s">
+      <c r="A42" s="27"/>
+      <c r="B42" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C42" s="35">
+      <c r="C42" s="36">
         <f>AVERAGE(D42,D43,D44)</f>
         <v>45.381666666666661</v>
       </c>
@@ -3686,9 +3837,9 @@
       </c>
     </row>
     <row r="43" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="36"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="35"/>
+      <c r="A43" s="27"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="36"/>
       <c r="D43" s="19">
         <v>44.512999999999998</v>
       </c>
@@ -3718,9 +3869,9 @@
       </c>
     </row>
     <row r="44" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="36"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="35"/>
+      <c r="A44" s="27"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="36"/>
       <c r="D44" s="21">
         <v>44.231999999999999</v>
       </c>
@@ -3750,7 +3901,7 @@
       </c>
     </row>
     <row r="45" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="27" t="s">
         <v>112</v>
       </c>
       <c r="B45" s="12" t="s">
@@ -3786,7 +3937,7 @@
       </c>
     </row>
     <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="36"/>
+      <c r="A46" s="27"/>
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="8"/>
@@ -3800,11 +3951,11 @@
       <c r="L46" s="9"/>
     </row>
     <row r="47" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="36"/>
-      <c r="B47" s="34" t="s">
+      <c r="A47" s="27"/>
+      <c r="B47" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C47" s="35">
+      <c r="C47" s="36">
         <f>AVERAGE(D47:D49)</f>
         <v>43.773500000000006</v>
       </c>
@@ -3837,9 +3988,9 @@
       </c>
     </row>
     <row r="48" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="36"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="35"/>
+      <c r="A48" s="27"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
       <c r="D48" s="19">
         <v>44.283999999999999</v>
       </c>
@@ -3869,9 +4020,9 @@
       </c>
     </row>
     <row r="49" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="36"/>
-      <c r="B49" s="34"/>
-      <c r="C49" s="35"/>
+      <c r="A49" s="27"/>
+      <c r="B49" s="35"/>
+      <c r="C49" s="36"/>
       <c r="D49" s="21">
         <v>45.834000000000003</v>
       </c>
@@ -3901,7 +4052,7 @@
       </c>
     </row>
     <row r="50" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="36" t="s">
+      <c r="A50" s="27" t="s">
         <v>113</v>
       </c>
       <c r="B50" s="12" t="s">
@@ -3937,7 +4088,7 @@
       </c>
     </row>
     <row r="51" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="36"/>
+      <c r="A51" s="27"/>
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="8"/>
@@ -3951,11 +4102,11 @@
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="36"/>
-      <c r="B52" s="39" t="s">
+      <c r="A52" s="27"/>
+      <c r="B52" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C52" s="42">
+      <c r="C52" s="37">
         <f>AVERAGE(D52,D53,D54)</f>
         <v>26.851500000000001</v>
       </c>
@@ -3988,9 +4139,9 @@
       </c>
     </row>
     <row r="53" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="36"/>
-      <c r="B53" s="40"/>
-      <c r="C53" s="43"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="41"/>
+      <c r="C53" s="38"/>
       <c r="D53" s="19">
         <v>26.452999999999999</v>
       </c>
@@ -4020,9 +4171,9 @@
       </c>
     </row>
     <row r="54" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="36"/>
-      <c r="B54" s="41"/>
-      <c r="C54" s="44"/>
+      <c r="A54" s="27"/>
+      <c r="B54" s="42"/>
+      <c r="C54" s="39"/>
       <c r="D54" s="21">
         <v>28.149000000000001</v>
       </c>
@@ -4052,7 +4203,7 @@
       </c>
     </row>
     <row r="55" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="36" t="s">
+      <c r="A55" s="27" t="s">
         <v>114</v>
       </c>
       <c r="B55" s="12" t="s">
@@ -4088,7 +4239,7 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="36"/>
+      <c r="A56" s="27"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="8"/>
@@ -4102,11 +4253,11 @@
       <c r="L56" s="9"/>
     </row>
     <row r="57" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="36"/>
-      <c r="B57" s="34" t="s">
+      <c r="A57" s="27"/>
+      <c r="B57" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C57" s="35">
+      <c r="C57" s="36">
         <f>AVERAGE(D57,D58,D59)</f>
         <v>48.290166666666664</v>
       </c>
@@ -4139,9 +4290,9 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="36"/>
-      <c r="B58" s="34"/>
-      <c r="C58" s="35"/>
+      <c r="A58" s="27"/>
+      <c r="B58" s="35"/>
+      <c r="C58" s="36"/>
       <c r="D58" s="19">
         <v>48.340499999999999</v>
       </c>
@@ -4171,9 +4322,9 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="36"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="35"/>
+      <c r="A59" s="27"/>
+      <c r="B59" s="35"/>
+      <c r="C59" s="36"/>
       <c r="D59" s="21">
         <v>48.305999999999997</v>
       </c>
@@ -4203,7 +4354,7 @@
       </c>
     </row>
     <row r="60" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="36" t="s">
+      <c r="A60" s="27" t="s">
         <v>262</v>
       </c>
       <c r="B60" s="12" t="s">
@@ -4239,7 +4390,7 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="36"/>
+      <c r="A61" s="27"/>
       <c r="B61" s="12"/>
       <c r="C61" s="12"/>
       <c r="D61" s="8"/>
@@ -4253,11 +4404,11 @@
       <c r="L61" s="9"/>
     </row>
     <row r="62" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="36"/>
-      <c r="B62" s="34" t="s">
+      <c r="A62" s="27"/>
+      <c r="B62" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C62" s="35">
+      <c r="C62" s="36">
         <f>AVERAGE(D62,D63,D64)</f>
         <v>48.94466666666667</v>
       </c>
@@ -4290,9 +4441,9 @@
       </c>
     </row>
     <row r="63" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="36"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="35"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="35"/>
+      <c r="C63" s="36"/>
       <c r="D63" s="19">
         <v>48.736499999999999</v>
       </c>
@@ -4322,9 +4473,9 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="36"/>
-      <c r="B64" s="34"/>
-      <c r="C64" s="35"/>
+      <c r="A64" s="27"/>
+      <c r="B64" s="35"/>
+      <c r="C64" s="36"/>
       <c r="D64" s="21">
         <v>49.253</v>
       </c>
@@ -4368,7 +4519,7 @@
       <c r="L65" s="26"/>
     </row>
     <row r="66" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="36" t="s">
+      <c r="A66" s="27" t="s">
         <v>378</v>
       </c>
       <c r="B66" s="28" t="s">
@@ -4407,7 +4558,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="36"/>
+      <c r="A67" s="27"/>
       <c r="B67" s="29"/>
       <c r="C67" s="29"/>
       <c r="D67" s="8">
@@ -4439,7 +4590,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="36"/>
+      <c r="A68" s="27"/>
       <c r="B68" s="30"/>
       <c r="C68" s="30"/>
       <c r="D68" s="8">
@@ -4471,11 +4622,11 @@
       </c>
     </row>
     <row r="69" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="36"/>
-      <c r="B69" s="34" t="s">
+      <c r="A69" s="27"/>
+      <c r="B69" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C69" s="35">
+      <c r="C69" s="36">
         <f>AVERAGE(D69:D71)</f>
         <v>53.914666666666669</v>
       </c>
@@ -4508,9 +4659,9 @@
       </c>
     </row>
     <row r="70" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="36"/>
-      <c r="B70" s="34"/>
-      <c r="C70" s="35"/>
+      <c r="A70" s="27"/>
+      <c r="B70" s="35"/>
+      <c r="C70" s="36"/>
       <c r="D70" s="19">
         <v>53.600499999999997</v>
       </c>
@@ -4540,9 +4691,9 @@
       </c>
     </row>
     <row r="71" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="36"/>
-      <c r="B71" s="34"/>
-      <c r="C71" s="35"/>
+      <c r="A71" s="27"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="36"/>
       <c r="D71" s="21">
         <v>54.435499999999998</v>
       </c>
@@ -4572,7 +4723,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="36" t="s">
+      <c r="A72" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B72" s="28" t="s">
@@ -4611,7 +4762,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="36"/>
+      <c r="A73" s="27"/>
       <c r="B73" s="29"/>
       <c r="C73" s="32"/>
       <c r="D73" s="8">
@@ -4643,9 +4794,9 @@
       </c>
     </row>
     <row r="74" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="36"/>
+      <c r="A74" s="27"/>
       <c r="B74" s="30"/>
-      <c r="C74" s="33"/>
+      <c r="C74" s="34"/>
       <c r="D74" s="8">
         <v>43.276499999999999</v>
       </c>
@@ -4675,11 +4826,11 @@
       </c>
     </row>
     <row r="75" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="36"/>
-      <c r="B75" s="34" t="s">
+      <c r="A75" s="27"/>
+      <c r="B75" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C75" s="35">
+      <c r="C75" s="36">
         <f>AVERAGE(D75:D77)</f>
         <v>45.364333333333327</v>
       </c>
@@ -4712,9 +4863,9 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="36"/>
-      <c r="B76" s="34"/>
-      <c r="C76" s="35"/>
+      <c r="A76" s="27"/>
+      <c r="B76" s="35"/>
+      <c r="C76" s="36"/>
       <c r="D76" s="19">
         <v>45.332999999999998</v>
       </c>
@@ -4744,9 +4895,9 @@
       </c>
     </row>
     <row r="77" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="36"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="35"/>
+      <c r="A77" s="27"/>
+      <c r="B77" s="35"/>
+      <c r="C77" s="36"/>
       <c r="D77" s="21">
         <v>44.664999999999999</v>
       </c>
@@ -4776,7 +4927,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="36" t="s">
+      <c r="A78" s="27" t="s">
         <v>116</v>
       </c>
       <c r="B78" s="28" t="s">
@@ -4815,7 +4966,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="36"/>
+      <c r="A79" s="27"/>
       <c r="B79" s="29"/>
       <c r="C79" s="32"/>
       <c r="D79" s="8">
@@ -4847,9 +4998,9 @@
       </c>
     </row>
     <row r="80" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="36"/>
+      <c r="A80" s="27"/>
       <c r="B80" s="30"/>
-      <c r="C80" s="33"/>
+      <c r="C80" s="34"/>
       <c r="D80" s="8">
         <v>60.000999999999998</v>
       </c>
@@ -4879,11 +5030,11 @@
       </c>
     </row>
     <row r="81" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="36"/>
-      <c r="B81" s="34" t="s">
+      <c r="A81" s="27"/>
+      <c r="B81" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C81" s="35">
+      <c r="C81" s="36">
         <f>AVERAGE(D81:D83)</f>
         <v>60.632333333333328</v>
       </c>
@@ -4916,9 +5067,9 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="36"/>
-      <c r="B82" s="34"/>
-      <c r="C82" s="35"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="35"/>
+      <c r="C82" s="36"/>
       <c r="D82" s="19">
         <v>60.64</v>
       </c>
@@ -4948,9 +5099,9 @@
       </c>
     </row>
     <row r="83" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="36"/>
-      <c r="B83" s="34"/>
-      <c r="C83" s="35"/>
+      <c r="A83" s="27"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="36"/>
       <c r="D83" s="21">
         <v>61.267000000000003</v>
       </c>
@@ -4980,7 +5131,7 @@
       </c>
     </row>
     <row r="84" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="27" t="s">
         <v>383</v>
       </c>
       <c r="B84" s="28" t="s">
@@ -5019,7 +5170,7 @@
       </c>
     </row>
     <row r="85" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="36"/>
+      <c r="A85" s="27"/>
       <c r="B85" s="29"/>
       <c r="C85" s="32"/>
       <c r="D85" s="8">
@@ -5051,9 +5202,9 @@
       </c>
     </row>
     <row r="86" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="36"/>
+      <c r="A86" s="27"/>
       <c r="B86" s="30"/>
-      <c r="C86" s="33"/>
+      <c r="C86" s="34"/>
       <c r="D86" s="8">
         <v>59.4345</v>
       </c>
@@ -5083,11 +5234,11 @@
       </c>
     </row>
     <row r="87" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="36"/>
-      <c r="B87" s="34" t="s">
+      <c r="A87" s="27"/>
+      <c r="B87" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C87" s="35">
+      <c r="C87" s="36">
         <f>AVERAGE(D87:D89)</f>
         <v>55.1175</v>
       </c>
@@ -5120,9 +5271,9 @@
       </c>
     </row>
     <row r="88" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="36"/>
-      <c r="B88" s="34"/>
-      <c r="C88" s="35"/>
+      <c r="A88" s="27"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="36"/>
       <c r="D88" s="19">
         <v>53.138500000000001</v>
       </c>
@@ -5152,9 +5303,9 @@
       </c>
     </row>
     <row r="89" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="36"/>
-      <c r="B89" s="34"/>
-      <c r="C89" s="35"/>
+      <c r="A89" s="27"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="36"/>
       <c r="D89" s="21">
         <v>58.354500000000002</v>
       </c>
@@ -5184,7 +5335,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="36" t="s">
+      <c r="A90" s="27" t="s">
         <v>386</v>
       </c>
       <c r="B90" s="28" t="s">
@@ -5223,7 +5374,7 @@
       </c>
     </row>
     <row r="91" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="36"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="29"/>
       <c r="C91" s="32"/>
       <c r="D91" s="8">
@@ -5255,9 +5406,9 @@
       </c>
     </row>
     <row r="92" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="36"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="30"/>
-      <c r="C92" s="33"/>
+      <c r="C92" s="34"/>
       <c r="D92" s="8">
         <v>58.045499999999997</v>
       </c>
@@ -5287,11 +5438,11 @@
       </c>
     </row>
     <row r="93" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="36"/>
-      <c r="B93" s="34" t="s">
+      <c r="A93" s="27"/>
+      <c r="B93" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C93" s="35">
+      <c r="C93" s="36">
         <f>AVERAGE(D93:D95)</f>
         <v>58.660166666666669</v>
       </c>
@@ -5324,9 +5475,9 @@
       </c>
     </row>
     <row r="94" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="36"/>
-      <c r="B94" s="34"/>
-      <c r="C94" s="35"/>
+      <c r="A94" s="27"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="36"/>
       <c r="D94" s="19">
         <v>58.539499999999997</v>
       </c>
@@ -5356,9 +5507,9 @@
       </c>
     </row>
     <row r="95" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="36"/>
-      <c r="B95" s="34"/>
-      <c r="C95" s="35"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="36"/>
       <c r="D95" s="21">
         <v>58.933</v>
       </c>
@@ -5388,7 +5539,7 @@
       </c>
     </row>
     <row r="96" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="36" t="s">
+      <c r="A96" s="27" t="s">
         <v>138</v>
       </c>
       <c r="B96" s="28" t="s">
@@ -5427,7 +5578,7 @@
       </c>
     </row>
     <row r="97" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="36"/>
+      <c r="A97" s="27"/>
       <c r="B97" s="29"/>
       <c r="C97" s="32"/>
       <c r="D97" s="8">
@@ -5459,9 +5610,9 @@
       </c>
     </row>
     <row r="98" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="36"/>
+      <c r="A98" s="27"/>
       <c r="B98" s="30"/>
-      <c r="C98" s="33"/>
+      <c r="C98" s="34"/>
       <c r="D98" s="8">
         <v>63.207000000000001</v>
       </c>
@@ -5491,11 +5642,11 @@
       </c>
     </row>
     <row r="99" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="36"/>
-      <c r="B99" s="34" t="s">
+      <c r="A99" s="27"/>
+      <c r="B99" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C99" s="35">
+      <c r="C99" s="36">
         <f>AVERAGE(D99:D101)</f>
         <v>62.750333333333323</v>
       </c>
@@ -5528,9 +5679,9 @@
       </c>
     </row>
     <row r="100" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="36"/>
-      <c r="B100" s="34"/>
-      <c r="C100" s="35"/>
+      <c r="A100" s="27"/>
+      <c r="B100" s="35"/>
+      <c r="C100" s="36"/>
       <c r="D100" s="19">
         <v>63.038499999999999</v>
       </c>
@@ -5560,9 +5711,9 @@
       </c>
     </row>
     <row r="101" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="36"/>
-      <c r="B101" s="34"/>
-      <c r="C101" s="35"/>
+      <c r="A101" s="27"/>
+      <c r="B101" s="35"/>
+      <c r="C101" s="36"/>
       <c r="D101" s="21">
         <v>62.92</v>
       </c>
@@ -5592,7 +5743,7 @@
       </c>
     </row>
     <row r="102" spans="1:12" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="36" t="s">
+      <c r="A102" s="27" t="s">
         <v>139</v>
       </c>
       <c r="B102" s="12" t="s">
@@ -5628,7 +5779,7 @@
       </c>
     </row>
     <row r="103" spans="1:12" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="36"/>
+      <c r="A103" s="27"/>
       <c r="B103" s="12"/>
       <c r="C103" s="12"/>
       <c r="D103" s="8"/>
@@ -5642,9 +5793,9 @@
       <c r="L103" s="9"/>
     </row>
     <row r="104" spans="1:12" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="36"/>
-      <c r="B104" s="34"/>
-      <c r="C104" s="34"/>
+      <c r="A104" s="27"/>
+      <c r="B104" s="35"/>
+      <c r="C104" s="35"/>
       <c r="D104" s="19"/>
       <c r="E104" s="20"/>
       <c r="F104" s="20"/>
@@ -5656,9 +5807,9 @@
       <c r="L104" s="20"/>
     </row>
     <row r="105" spans="1:12" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="36"/>
-      <c r="B105" s="34"/>
-      <c r="C105" s="34"/>
+      <c r="A105" s="27"/>
+      <c r="B105" s="35"/>
+      <c r="C105" s="35"/>
       <c r="D105" s="19">
         <v>50.713500000000003</v>
       </c>
@@ -5688,11 +5839,11 @@
       </c>
     </row>
     <row r="106" spans="1:12" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="36"/>
-      <c r="B106" s="34" t="s">
+      <c r="A106" s="27"/>
+      <c r="B106" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C106" s="34"/>
+      <c r="C106" s="35"/>
       <c r="D106" s="21">
         <v>60.002000000000002</v>
       </c>
@@ -5722,7 +5873,7 @@
       </c>
     </row>
     <row r="107" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A107" s="36" t="s">
+      <c r="A107" s="27" t="s">
         <v>510</v>
       </c>
       <c r="B107" s="28" t="s">
@@ -5761,7 +5912,7 @@
       </c>
     </row>
     <row r="108" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A108" s="36"/>
+      <c r="A108" s="27"/>
       <c r="B108" s="29"/>
       <c r="C108" s="32"/>
       <c r="D108" s="7">
@@ -5793,9 +5944,9 @@
       </c>
     </row>
     <row r="109" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A109" s="36"/>
+      <c r="A109" s="27"/>
       <c r="B109" s="29"/>
-      <c r="C109" s="45"/>
+      <c r="C109" s="33"/>
       <c r="D109" s="2">
         <v>21.6205</v>
       </c>
@@ -5825,9 +5976,9 @@
       </c>
     </row>
     <row r="110" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A110" s="36"/>
+      <c r="A110" s="27"/>
       <c r="B110" s="30"/>
-      <c r="C110" s="33"/>
+      <c r="C110" s="34"/>
       <c r="D110" s="4">
         <v>26.020499999999998</v>
       </c>
@@ -5857,11 +6008,11 @@
       </c>
     </row>
     <row r="111" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A111" s="36"/>
-      <c r="B111" s="34" t="s">
+      <c r="A111" s="27"/>
+      <c r="B111" s="35" t="s">
         <v>264</v>
       </c>
-      <c r="C111" s="35">
+      <c r="C111" s="36">
         <f>AVERAGE(D111:D116)</f>
         <v>23.628916666666665</v>
       </c>
@@ -5894,9 +6045,9 @@
       </c>
     </row>
     <row r="112" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A112" s="36"/>
-      <c r="B112" s="34"/>
-      <c r="C112" s="35"/>
+      <c r="A112" s="27"/>
+      <c r="B112" s="35"/>
+      <c r="C112" s="36"/>
       <c r="D112" s="19">
         <v>18.373999999999999</v>
       </c>
@@ -5926,9 +6077,9 @@
       </c>
     </row>
     <row r="113" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="36"/>
-      <c r="B113" s="34"/>
-      <c r="C113" s="35"/>
+      <c r="A113" s="27"/>
+      <c r="B113" s="35"/>
+      <c r="C113" s="36"/>
       <c r="D113" s="21">
         <v>25.271999999999998</v>
       </c>
@@ -6063,7 +6214,7 @@
       <c r="A121" s="11"/>
     </row>
     <row r="122" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A122" s="36" t="s">
+      <c r="A122" s="27" t="s">
         <v>115</v>
       </c>
       <c r="B122" s="28" t="s">
@@ -6102,7 +6253,7 @@
       </c>
     </row>
     <row r="123" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A123" s="36"/>
+      <c r="A123" s="27"/>
       <c r="B123" s="29"/>
       <c r="C123" s="32"/>
       <c r="D123" s="8">
@@ -6134,9 +6285,9 @@
       </c>
     </row>
     <row r="124" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A124" s="36"/>
+      <c r="A124" s="27"/>
       <c r="B124" s="30"/>
-      <c r="C124" s="33"/>
+      <c r="C124" s="34"/>
       <c r="D124" s="8">
         <v>43.276499999999999</v>
       </c>
@@ -6166,11 +6317,11 @@
       </c>
     </row>
     <row r="125" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A125" s="36"/>
-      <c r="B125" s="34" t="s">
+      <c r="A125" s="27"/>
+      <c r="B125" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C125" s="35">
+      <c r="C125" s="36">
         <f>AVERAGE(D125:D127)</f>
         <v>45.364333333333327</v>
       </c>
@@ -6203,9 +6354,9 @@
       </c>
     </row>
     <row r="126" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A126" s="36"/>
-      <c r="B126" s="34"/>
-      <c r="C126" s="35"/>
+      <c r="A126" s="27"/>
+      <c r="B126" s="35"/>
+      <c r="C126" s="36"/>
       <c r="D126" s="19">
         <v>45.332999999999998</v>
       </c>
@@ -6235,9 +6386,9 @@
       </c>
     </row>
     <row r="127" spans="1:12" ht="15" x14ac:dyDescent="0.15">
-      <c r="A127" s="36"/>
-      <c r="B127" s="34"/>
-      <c r="C127" s="35"/>
+      <c r="A127" s="27"/>
+      <c r="B127" s="35"/>
+      <c r="C127" s="36"/>
       <c r="D127" s="21">
         <v>44.664999999999999</v>
       </c>
@@ -6266,7 +6417,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="27" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A129" s="16" t="s">
         <v>101</v>
       </c>
@@ -6290,12 +6441,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A130" s="27" t="s">
-        <v>115</v>
+    <row r="130" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A130" s="45" t="s">
+        <v>616</v>
       </c>
       <c r="B130" s="28" t="s">
-        <v>140</v>
+        <v>614</v>
       </c>
       <c r="C130" s="31">
         <f>AVERAGE(D130:D132)</f>
@@ -6317,8 +6468,8 @@
         <v>574</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A131" s="27"/>
+    <row r="131" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A131" s="45"/>
       <c r="B131" s="29"/>
       <c r="C131" s="32"/>
       <c r="D131" s="9">
@@ -6337,10 +6488,10 @@
         <v>576</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="14.25" x14ac:dyDescent="0.15">
-      <c r="A132" s="27"/>
+    <row r="132" spans="1:12" ht="14.25" x14ac:dyDescent="0.15">
+      <c r="A132" s="45"/>
       <c r="B132" s="30"/>
-      <c r="C132" s="33"/>
+      <c r="C132" s="34"/>
       <c r="D132" s="9">
         <v>17.649999999999999</v>
       </c>
@@ -6357,12 +6508,12 @@
         <v>578</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A133" s="27"/>
-      <c r="B133" s="34" t="s">
+    <row r="133" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+      <c r="A133" s="45"/>
+      <c r="B133" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="C133" s="35">
+      <c r="C133" s="36">
         <f>AVERAGE(D133:D135)</f>
         <v>15.683333333333332</v>
       </c>
@@ -6382,10 +6533,10 @@
         <v>572</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A134" s="27"/>
-      <c r="B134" s="34"/>
-      <c r="C134" s="35"/>
+    <row r="134" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+      <c r="A134" s="45"/>
+      <c r="B134" s="35"/>
+      <c r="C134" s="36"/>
       <c r="D134" s="20">
         <v>15.42</v>
       </c>
@@ -6402,10 +6553,10 @@
         <v>580</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="15" x14ac:dyDescent="0.15">
-      <c r="A135" s="27"/>
-      <c r="B135" s="34"/>
-      <c r="C135" s="35"/>
+    <row r="135" spans="1:12" ht="15" x14ac:dyDescent="0.15">
+      <c r="A135" s="45"/>
+      <c r="B135" s="35"/>
+      <c r="C135" s="36"/>
       <c r="D135" s="22">
         <v>15.73</v>
       </c>
@@ -6422,27 +6573,277 @@
         <v>582</v>
       </c>
     </row>
+    <row r="136" spans="1:12" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="137" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="47" t="s">
+        <v>617</v>
+      </c>
+      <c r="B137" s="40" t="s">
+        <v>615</v>
+      </c>
+      <c r="C137" s="37">
+        <f>AVERAGE(D137:D141)</f>
+        <v>14.018000000000001</v>
+      </c>
+      <c r="D137" s="20">
+        <v>13.31</v>
+      </c>
+      <c r="E137" s="20">
+        <v>12.53</v>
+      </c>
+      <c r="F137" s="19">
+        <v>43.76</v>
+      </c>
+      <c r="G137" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="H137" s="20" t="s">
+        <v>587</v>
+      </c>
+      <c r="I137" s="46" t="s">
+        <v>409</v>
+      </c>
+      <c r="J137" s="46" t="s">
+        <v>588</v>
+      </c>
+      <c r="K137" s="46" t="s">
+        <v>589</v>
+      </c>
+      <c r="L137" s="46" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="48"/>
+      <c r="B138" s="41"/>
+      <c r="C138" s="38"/>
+      <c r="D138" s="20">
+        <v>14.27</v>
+      </c>
+      <c r="E138" s="20">
+        <v>12.81</v>
+      </c>
+      <c r="F138" s="19">
+        <v>34.03</v>
+      </c>
+      <c r="G138" s="20" t="s">
+        <v>591</v>
+      </c>
+      <c r="H138" s="20" t="s">
+        <v>592</v>
+      </c>
+      <c r="I138" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="J138" s="46" t="s">
+        <v>593</v>
+      </c>
+      <c r="K138" s="46" t="s">
+        <v>594</v>
+      </c>
+      <c r="L138" s="46" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="48"/>
+      <c r="B139" s="41"/>
+      <c r="C139" s="38"/>
+      <c r="D139" s="22">
+        <v>14.57</v>
+      </c>
+      <c r="E139" s="22">
+        <v>13.39</v>
+      </c>
+      <c r="F139" s="21">
+        <v>28.11</v>
+      </c>
+      <c r="G139" s="22" t="s">
+        <v>596</v>
+      </c>
+      <c r="H139" s="22" t="s">
+        <v>597</v>
+      </c>
+      <c r="I139" s="46" t="s">
+        <v>168</v>
+      </c>
+      <c r="J139" s="46" t="s">
+        <v>598</v>
+      </c>
+      <c r="K139" s="46" t="s">
+        <v>599</v>
+      </c>
+      <c r="L139" s="46" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="48"/>
+      <c r="B140" s="41"/>
+      <c r="C140" s="38"/>
+      <c r="D140" s="20">
+        <v>14.03</v>
+      </c>
+      <c r="E140" s="20">
+        <v>13.16</v>
+      </c>
+      <c r="F140" s="19">
+        <v>39.03</v>
+      </c>
+      <c r="G140" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="H140" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="I140" s="46" t="s">
+        <v>602</v>
+      </c>
+      <c r="J140" s="46" t="s">
+        <v>603</v>
+      </c>
+      <c r="K140" s="46" t="s">
+        <v>604</v>
+      </c>
+      <c r="L140" s="46" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="48"/>
+      <c r="B141" s="42"/>
+      <c r="C141" s="39"/>
+      <c r="D141" s="20">
+        <v>13.91</v>
+      </c>
+      <c r="E141" s="20">
+        <v>13.61</v>
+      </c>
+      <c r="F141" s="19">
+        <v>37.49</v>
+      </c>
+      <c r="G141" s="20" t="s">
+        <v>613</v>
+      </c>
+      <c r="H141" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="I141" s="46" t="s">
+        <v>609</v>
+      </c>
+      <c r="J141" s="46" t="s">
+        <v>610</v>
+      </c>
+      <c r="K141" s="46" t="s">
+        <v>611</v>
+      </c>
+      <c r="L141" s="46" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A142" s="48"/>
+      <c r="B142" s="40" t="s">
+        <v>618</v>
+      </c>
+      <c r="C142" s="37" t="e">
+        <f>AVERAGE(D142:D146)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D142" s="20"/>
+      <c r="E142" s="20"/>
+      <c r="F142" s="19"/>
+      <c r="G142" s="20"/>
+      <c r="H142" s="20"/>
+    </row>
+    <row r="143" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A143" s="48"/>
+      <c r="B143" s="41"/>
+      <c r="C143" s="38"/>
+      <c r="D143" s="20"/>
+      <c r="E143" s="20"/>
+      <c r="F143" s="19"/>
+      <c r="G143" s="20"/>
+      <c r="H143" s="20"/>
+    </row>
+    <row r="144" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="48"/>
+      <c r="B144" s="41"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="22"/>
+      <c r="E144" s="22"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="22"/>
+      <c r="H144" s="22"/>
+    </row>
+    <row r="145" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="48"/>
+      <c r="B145" s="41"/>
+      <c r="C145" s="38"/>
+      <c r="D145" s="20"/>
+      <c r="E145" s="20"/>
+      <c r="F145" s="19"/>
+      <c r="G145" s="20"/>
+      <c r="H145" s="20"/>
+    </row>
+    <row r="146" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="48"/>
+      <c r="B146" s="42"/>
+      <c r="C146" s="39"/>
+      <c r="D146" s="20"/>
+      <c r="E146" s="20"/>
+      <c r="F146" s="19"/>
+      <c r="G146" s="20"/>
+      <c r="H146" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="76">
-    <mergeCell ref="A107:A113"/>
-    <mergeCell ref="B107:B110"/>
-    <mergeCell ref="C107:C110"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="C111:C113"/>
-    <mergeCell ref="C66:C68"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B90:B92"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B69:B71"/>
-    <mergeCell ref="C69:C71"/>
-    <mergeCell ref="C96:C98"/>
-    <mergeCell ref="C90:C92"/>
-    <mergeCell ref="C84:C86"/>
-    <mergeCell ref="C78:C80"/>
-    <mergeCell ref="C72:C74"/>
+  <mergeCells count="81">
+    <mergeCell ref="B142:B146"/>
+    <mergeCell ref="C142:C146"/>
+    <mergeCell ref="A137:A146"/>
+    <mergeCell ref="B137:B141"/>
+    <mergeCell ref="C137:C141"/>
+    <mergeCell ref="A130:A135"/>
+    <mergeCell ref="B130:B132"/>
+    <mergeCell ref="C130:C132"/>
+    <mergeCell ref="B133:B135"/>
+    <mergeCell ref="C133:C135"/>
+    <mergeCell ref="A122:A127"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="C122:C124"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="A60:A64"/>
+    <mergeCell ref="A66:A71"/>
+    <mergeCell ref="A72:A77"/>
+    <mergeCell ref="A78:A83"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="C62:C64"/>
+    <mergeCell ref="B62:B64"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="C57:C59"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="B47:B49"/>
+    <mergeCell ref="C47:C49"/>
+    <mergeCell ref="C52:C54"/>
     <mergeCell ref="A102:A106"/>
     <mergeCell ref="B75:B77"/>
     <mergeCell ref="C75:C77"/>
@@ -6459,47 +6860,25 @@
     <mergeCell ref="A96:A101"/>
     <mergeCell ref="A84:A89"/>
     <mergeCell ref="C104:C106"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="C52:C54"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="C57:C59"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A50:A54"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A44"/>
-    <mergeCell ref="A45:A49"/>
-    <mergeCell ref="A55:A59"/>
-    <mergeCell ref="A60:A64"/>
-    <mergeCell ref="A66:A71"/>
-    <mergeCell ref="A72:A77"/>
-    <mergeCell ref="A78:A83"/>
-    <mergeCell ref="A122:A127"/>
-    <mergeCell ref="B122:B124"/>
-    <mergeCell ref="C122:C124"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="A130:A135"/>
-    <mergeCell ref="B130:B132"/>
-    <mergeCell ref="C130:C132"/>
-    <mergeCell ref="B133:B135"/>
-    <mergeCell ref="C133:C135"/>
+    <mergeCell ref="C66:C68"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B90:B92"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B69:B71"/>
+    <mergeCell ref="C69:C71"/>
+    <mergeCell ref="C96:C98"/>
+    <mergeCell ref="C90:C92"/>
+    <mergeCell ref="C84:C86"/>
+    <mergeCell ref="C78:C80"/>
+    <mergeCell ref="C72:C74"/>
+    <mergeCell ref="A107:A113"/>
+    <mergeCell ref="B107:B110"/>
+    <mergeCell ref="C107:C110"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="C111:C113"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>